<commit_message>
.xls file is already uploading
</commit_message>
<xml_diff>
--- a/TestData/users_list.xlsx
+++ b/TestData/users_list.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>